<commit_message>
modifile jsp name page
</commit_message>
<xml_diff>
--- a/report_invoice.xlsx
+++ b/report_invoice.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="90">
   <si>
     <t>Invoice Date</t>
   </si>
@@ -32,169 +32,253 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>IV46</t>
-  </si>
-  <si>
-    <t>2025-03-13</t>
+    <t>IV1</t>
+  </si>
+  <si>
+    <t>2025-01-30</t>
+  </si>
+  <si>
+    <t>Dịch vụ tháng 1/2025</t>
+  </si>
+  <si>
+    <t>Bob Tran</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>IV10</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>A018</t>
+  </si>
+  <si>
+    <t>IV11</t>
+  </si>
+  <si>
+    <t>Quang</t>
+  </si>
+  <si>
+    <t>A019</t>
+  </si>
+  <si>
+    <t>IV12</t>
+  </si>
+  <si>
+    <t>Henry Do</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>IV13</t>
+  </si>
+  <si>
+    <t>Luân</t>
+  </si>
+  <si>
+    <t>A020</t>
+  </si>
+  <si>
+    <t>IV14</t>
+  </si>
+  <si>
+    <t>Jack Le</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>IV15</t>
+  </si>
+  <si>
+    <t>David Pham</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>IV16</t>
+  </si>
+  <si>
+    <t>Grace Ly</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>IV17</t>
+  </si>
+  <si>
+    <t>Eve Hoang</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>IV18</t>
+  </si>
+  <si>
+    <t>Ivy Nguyen</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>IV19</t>
+  </si>
+  <si>
+    <t>Charlie Le</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>IV2</t>
+  </si>
+  <si>
+    <t>me cua thanh</t>
+  </si>
+  <si>
+    <t>A011</t>
+  </si>
+  <si>
+    <t>IV20</t>
+  </si>
+  <si>
+    <t>Frank Vu</t>
+  </si>
+  <si>
+    <t>A009</t>
+  </si>
+  <si>
+    <t>IV21</t>
+  </si>
+  <si>
+    <t>2025-02-28</t>
+  </si>
+  <si>
+    <t>Dịch vụ tháng 2/2025</t>
+  </si>
+  <si>
+    <t>IV22</t>
+  </si>
+  <si>
+    <t>IV23</t>
+  </si>
+  <si>
+    <t>A012</t>
+  </si>
+  <si>
+    <t>IV24</t>
+  </si>
+  <si>
+    <t>A013</t>
+  </si>
+  <si>
+    <t>IV25</t>
+  </si>
+  <si>
+    <t>A010</t>
+  </si>
+  <si>
+    <t>IV26</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>A014</t>
+  </si>
+  <si>
+    <t>IV27</t>
+  </si>
+  <si>
+    <t>2323123</t>
+  </si>
+  <si>
+    <t>A015</t>
+  </si>
+  <si>
+    <t>IV28</t>
+  </si>
+  <si>
+    <t>A016</t>
+  </si>
+  <si>
+    <t>IV29</t>
+  </si>
+  <si>
+    <t>A017</t>
+  </si>
+  <si>
+    <t>IV3</t>
+  </si>
+  <si>
+    <t>IV30</t>
+  </si>
+  <si>
+    <t>IV31</t>
+  </si>
+  <si>
+    <t>IV32</t>
+  </si>
+  <si>
+    <t>IV33</t>
+  </si>
+  <si>
+    <t>IV34</t>
+  </si>
+  <si>
+    <t>IV35</t>
+  </si>
+  <si>
+    <t>IV36</t>
+  </si>
+  <si>
+    <t>IV37</t>
+  </si>
+  <si>
+    <t>IV38</t>
+  </si>
+  <si>
+    <t>IV39</t>
+  </si>
+  <si>
+    <t>IV4</t>
+  </si>
+  <si>
+    <t>IV40</t>
+  </si>
+  <si>
+    <t>IV41</t>
+  </si>
+  <si>
+    <t>2025-03-27</t>
   </si>
   <si>
     <t>Dich vu thang 3</t>
   </si>
   <si>
-    <t>Bob Tran</t>
-  </si>
-  <si>
-    <t>A10_04</t>
-  </si>
-  <si>
-    <t>IV47</t>
-  </si>
-  <si>
-    <t>New User</t>
-  </si>
-  <si>
-    <t>A01_01</t>
-  </si>
-  <si>
-    <t>IV48</t>
-  </si>
-  <si>
-    <t>Charlie Le</t>
-  </si>
-  <si>
-    <t>A09_01</t>
-  </si>
-  <si>
-    <t>IV49</t>
-  </si>
-  <si>
-    <t>Eve Hoang</t>
-  </si>
-  <si>
-    <t>A10_01</t>
-  </si>
-  <si>
-    <t>IV50</t>
-  </si>
-  <si>
-    <t>Frank Vu</t>
-  </si>
-  <si>
-    <t>A11_02</t>
-  </si>
-  <si>
-    <t>IV51</t>
-  </si>
-  <si>
-    <t>David Pham</t>
-  </si>
-  <si>
-    <t>A11_03</t>
-  </si>
-  <si>
-    <t>IV52</t>
-  </si>
-  <si>
-    <t>A09_04</t>
-  </si>
-  <si>
-    <t>IV53</t>
-  </si>
-  <si>
-    <t>Henry Do</t>
-  </si>
-  <si>
-    <t>A09_03</t>
-  </si>
-  <si>
-    <t>IV54</t>
-  </si>
-  <si>
-    <t>Jack Le</t>
-  </si>
-  <si>
-    <t>A10_06</t>
-  </si>
-  <si>
-    <t>IV55</t>
-  </si>
-  <si>
-    <t>IV56</t>
-  </si>
-  <si>
-    <t>IV57</t>
-  </si>
-  <si>
-    <t>IV58</t>
-  </si>
-  <si>
-    <t>IV59</t>
-  </si>
-  <si>
-    <t>IV60</t>
-  </si>
-  <si>
-    <t>IV61</t>
-  </si>
-  <si>
-    <t>IV62</t>
-  </si>
-  <si>
-    <t>IV63</t>
-  </si>
-  <si>
-    <t>IV64</t>
-  </si>
-  <si>
-    <t>IV65</t>
-  </si>
-  <si>
-    <t>IV66</t>
-  </si>
-  <si>
-    <t>IV67</t>
-  </si>
-  <si>
-    <t>IV68</t>
-  </si>
-  <si>
-    <t>IV69</t>
-  </si>
-  <si>
-    <t>IV70</t>
-  </si>
-  <si>
-    <t>IV71</t>
-  </si>
-  <si>
-    <t>IV72</t>
-  </si>
-  <si>
-    <t>IV73</t>
-  </si>
-  <si>
-    <t>IV74</t>
-  </si>
-  <si>
-    <t>IV75</t>
-  </si>
-  <si>
-    <t>IV76</t>
-  </si>
-  <si>
-    <t>IV77</t>
-  </si>
-  <si>
-    <t>IV78</t>
-  </si>
-  <si>
-    <t>IV79</t>
-  </si>
-  <si>
-    <t>IV80</t>
-  </si>
-  <si>
-    <t>IV81</t>
+    <t>IV44</t>
+  </si>
+  <si>
+    <t>IV5</t>
+  </si>
+  <si>
+    <t>IV6</t>
+  </si>
+  <si>
+    <t>IV7</t>
+  </si>
+  <si>
+    <t>IV8</t>
+  </si>
+  <si>
+    <t>IV9</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -242,7 +326,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -250,10 +334,10 @@
   <cols>
     <col min="1" max="1" width="10.9140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.13671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.34375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.4921875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="18.10546875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.9140625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.65625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="9.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.9296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -293,7 +377,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>1.04962928E8</v>
+        <v>958167.0</v>
       </c>
     </row>
     <row r="3">
@@ -313,7 +397,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>1.7102824E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="4">
@@ -333,7 +417,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>1.6364224E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="5">
@@ -353,7 +437,7 @@
         <v>19</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="6">
@@ -373,7 +457,7 @@
         <v>22</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="7">
@@ -393,7 +477,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="8">
@@ -407,18 +491,18 @@
         <v>8</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>7</v>
@@ -427,18 +511,18 @@
         <v>8</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>7</v>
@@ -447,18 +531,18 @@
         <v>8</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>7</v>
@@ -467,18 +551,18 @@
         <v>8</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>1.04962928E8</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>7</v>
@@ -487,18 +571,18 @@
         <v>8</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>1.7102824E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s" s="0">
         <v>7</v>
@@ -507,18 +591,18 @@
         <v>8</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>1.6364224E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s" s="0">
         <v>7</v>
@@ -527,198 +611,198 @@
         <v>8</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>2462324.0</v>
+        <v>758167.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="F18" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="F19" t="n" s="0">
-        <v>2462324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="F20" t="n" s="0">
-        <v>1.05012928E8</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="F21" t="n" s="0">
-        <v>1.7152824E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="F22" t="n" s="0">
-        <v>1.6414224E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F23" t="n" s="0">
-        <v>2512324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>7</v>
@@ -727,218 +811,218 @@
         <v>8</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F24" t="n" s="0">
-        <v>2512324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F25" t="n" s="0">
-        <v>2512324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s" s="0">
         <v>15</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F26" t="n" s="0">
-        <v>2512324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F27" t="n" s="0">
-        <v>2512324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F28" t="n" s="0">
-        <v>2512324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F29" t="n" s="0">
-        <v>1.05002928E8</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F30" t="n" s="0">
-        <v>1.7142824E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F31" t="n" s="0">
-        <v>1.6404224E7</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F32" t="n" s="0">
-        <v>2502324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F33" t="n" s="0">
-        <v>2502324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F34" t="n" s="0">
-        <v>2502324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s" s="0">
         <v>7</v>
@@ -947,61 +1031,181 @@
         <v>8</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F35" t="n" s="0">
-        <v>2502324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F36" t="n" s="0">
-        <v>2502324.0</v>
+        <v>258167.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n" s="0">
-        <v>2502324.0</v>
+        <v>2531500.0</v>
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>42</v>
+      </c>
       <c r="E38" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="F38" t="n" s="0">
+        <v>1650514.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>258167.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F40" t="n" s="0">
+        <v>258167.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="F38" t="n" s="0">
-        <v>6.13625664E8</v>
+      <c r="E41" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="F41" t="n" s="0">
+        <v>258167.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="F42" t="n" s="0">
+        <v>258167.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="F43" t="n" s="0">
+        <v>258167.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="F44" t="n" s="0">
+        <v>1.5708694E7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>